<commit_message>
Finished initial verions of fab files for 12-12 teensy 4.1 arena. Need to check orientations.
</commit_message>
<xml_diff>
--- a/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/BOM_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/BOM_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -80,37 +80,73 @@
     <t xml:space="preserve">Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1uF ceramic Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1,C2,C3,C4,C5,C6,C7,C8,C9,C10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1591</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10uF Electrolytic Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11,C13,C15,C17,C19,C21,C23,C25,C27,C29,C31,C33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD,D4xL5.4mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2992602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22uF Electrolytic Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C12,C14,C16,C18,C20,C22,C24,C26,C28,C30,C32,C34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2895280</t>
+    <t xml:space="preserve">33 Ohm resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R215,R62,R48,R75,R201,R173,R177,R222,R214,R147,R10,R212,R203,R168,R139,R91,R86,R135,R189,R234,R181,R141,R151,R9,R226,R74,R68,R44,R206,R163,R231,R8,R82,R194,R124,R70,R233,R42,R152,R184,R50,R133,R171,R107,R216,R127,R161,R136,R80,R193,R179,R43,R144,R160,R230,R191,R211,R90,R143,R92,R36,R200,R56,R123,R29,R197,R140,R110,R132,R49,R77,R145,R155,R217,R210,R223,R40,R32,R69,R15,R23,R187,R4,R100,R228,R108,R95,R122,R138,R84,R6,R182,R111,R53,R169,R166,R63,R224,R103,R118,R60,R128,R72,R22,R97,R89,R116,R115,R38,R18,R88,R12,R25,R196,R73,R58,R87,R126,R146,R209,R71,R104,R3,R45,R158,R188,R21,R174,R199,R195,R28,R51,R175,R205,R64,R79,R47,R221,R167,R130,R13,R232,R57,R106,R66,R26,R198,R7,R186,R27,R14,R59,R129,R61,R37,R93,R78,R101,R165,R213,R190,R172,R76,R33,R96,R114,R83,R98,R99,R67,R119,R30,R16,R229,R202,R41,R149,R19,R35,R121,R109,R227,R156,R102,R34,R17,R20,R11,R170,R192,R120,R65,R125,R113,R5,R24,R81,R112,R142,R94,R204,R225,R154,R176,R134,R178,R218,R185,R164,R54,R46,R117,R159,R162,R208,R219,R183,R180,R137,R148,R85,R52,R207,R105,R131,R153,R39,R220,R157,R31,R55,R150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1uF ceramic capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30,C67,C69,C48,C91,C5,C61,C26,C19,C39,C40,C76,C73,C2,C93,C60,C50,C25,C15,C46,C57,C84,C54,C64,C94,C47,C34,C11,C18,C89,C72,C88,C20,C29,C24,C82,C21,C41,C66,C63,C55,C37,C70,C83,C86,C1,C36,C13,C49,C28,C16,C51,C22,C90,C75,C53,C45,C85,C4,C14,C62,C32,C17,C92,C42,C35,C6,C80,C78,C58,C81,C43,C27,C23,C3,C9,C59,C71,C68,C10,C77,C87,C8,C38,C33,C12,C44,C74,C65,C56,C52,C7,C79,C31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LVC2G17DBVR dual Schmitt-trigger buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U36,U60,U33,U45,U20,U28,U2,U48,U38,U79,U62,U37,U63,U49,U26,U70,U76,U56,U53,U69,U29,U80,U30,U31,U25,U77,U41,U32,U46,U58,U35,U61,U65,U74,U27,U24,U81,U57,U39,U75,U44,U59,U47,U83,U68,U78,U23,U50,U19,U73,U72,U64,U42,U43,U66,U55,U71,U51,U67,U22,U40,U21,U52,U54,U34,U82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N-channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C165220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100uF ceramic capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C97,C98,C106,C102,C99,C105,C95,C96,C100,C104,C103,C101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7432790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level shifter TXB0108PWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U13,U6,U10,U3,U14,U4,U7,U12,U8,U9,U11,U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSSOP-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C53406</t>
   </si>
   <si>
     <t xml:space="preserve">4-Pin Connector, JST SM04B-SRSS-TB or similar</t>
@@ -125,16 +161,16 @@
     <t xml:space="preserve">C145956</t>
   </si>
   <si>
-    <t xml:space="preserve">MOSFET N-channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C165220</t>
+    <t xml:space="preserve">SN74LVC1G17DBVR single schmitt trigger buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U17,U16,U15,U18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7836</t>
   </si>
   <si>
     <t xml:space="preserve">200 Ohm resistor</t>
@@ -143,10 +179,7 @@
     <t xml:space="preserve">R1</t>
   </si>
   <si>
-    <t xml:space="preserve">0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17540</t>
+    <t xml:space="preserve">C25087</t>
   </si>
   <si>
     <t xml:space="preserve">20k Ohms resistor</t>
@@ -155,67 +188,37 @@
     <t xml:space="preserve">R2</t>
   </si>
   <si>
-    <t xml:space="preserve">C4328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300 Ohm resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3,R4,R5,R6,R7,R8,R9,R10,R11,R12,R13,R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level shifter TXB0108PWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1,U2,U3,U4,U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSSOP-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C53406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear Voltage Regulators (LDO) 5V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6,U7,U8,U9,U10,U11,U12,U13,U14,U15,U16,U17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TO-252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2980701</t>
+    <t xml:space="preserve">C25765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15x1 female header, 0.1in pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10,P12,P7,P9,P11,P5,P4,P1,P6,P8,P2,P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">through hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide Switch SPDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
   </si>
   <si>
     <t xml:space="preserve">DC Power Barrel Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">through hole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">global parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15x1 female header, 0.1in pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1,P2,P3,P4,P5,P6,P7,P8,P9,P10,P11,P12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slide Switch SPDT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
+    <t xml:space="preserve">J1, J4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teensy4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -281,11 +284,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -349,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -386,8 +400,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -467,16 +485,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="52.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.89"/>
@@ -505,7 +523,7 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -515,41 +533,41 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>10</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="1" t="n">
-        <v>12</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,30 +580,29 @@
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8"/>
+      <c r="E6" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -597,12 +614,1031 @@
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="0"/>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
+      <c r="AO7" s="0"/>
+      <c r="AP7" s="0"/>
+      <c r="AQ7" s="0"/>
+      <c r="AR7" s="0"/>
+      <c r="AS7" s="0"/>
+      <c r="AT7" s="0"/>
+      <c r="AU7" s="0"/>
+      <c r="AV7" s="0"/>
+      <c r="AW7" s="0"/>
+      <c r="AX7" s="0"/>
+      <c r="AY7" s="0"/>
+      <c r="AZ7" s="0"/>
+      <c r="BA7" s="0"/>
+      <c r="BB7" s="0"/>
+      <c r="BC7" s="0"/>
+      <c r="BD7" s="0"/>
+      <c r="BE7" s="0"/>
+      <c r="BF7" s="0"/>
+      <c r="BG7" s="0"/>
+      <c r="BH7" s="0"/>
+      <c r="BI7" s="0"/>
+      <c r="BJ7" s="0"/>
+      <c r="BK7" s="0"/>
+      <c r="BL7" s="0"/>
+      <c r="BM7" s="0"/>
+      <c r="BN7" s="0"/>
+      <c r="BO7" s="0"/>
+      <c r="BP7" s="0"/>
+      <c r="BQ7" s="0"/>
+      <c r="BR7" s="0"/>
+      <c r="BS7" s="0"/>
+      <c r="BT7" s="0"/>
+      <c r="BU7" s="0"/>
+      <c r="BV7" s="0"/>
+      <c r="BW7" s="0"/>
+      <c r="BX7" s="0"/>
+      <c r="BY7" s="0"/>
+      <c r="BZ7" s="0"/>
+      <c r="CA7" s="0"/>
+      <c r="CB7" s="0"/>
+      <c r="CC7" s="0"/>
+      <c r="CD7" s="0"/>
+      <c r="CE7" s="0"/>
+      <c r="CF7" s="0"/>
+      <c r="CG7" s="0"/>
+      <c r="CH7" s="0"/>
+      <c r="CI7" s="0"/>
+      <c r="CJ7" s="0"/>
+      <c r="CK7" s="0"/>
+      <c r="CL7" s="0"/>
+      <c r="CM7" s="0"/>
+      <c r="CN7" s="0"/>
+      <c r="CO7" s="0"/>
+      <c r="CP7" s="0"/>
+      <c r="CQ7" s="0"/>
+      <c r="CR7" s="0"/>
+      <c r="CS7" s="0"/>
+      <c r="CT7" s="0"/>
+      <c r="CU7" s="0"/>
+      <c r="CV7" s="0"/>
+      <c r="CW7" s="0"/>
+      <c r="CX7" s="0"/>
+      <c r="CY7" s="0"/>
+      <c r="CZ7" s="0"/>
+      <c r="DA7" s="0"/>
+      <c r="DB7" s="0"/>
+      <c r="DC7" s="0"/>
+      <c r="DD7" s="0"/>
+      <c r="DE7" s="0"/>
+      <c r="DF7" s="0"/>
+      <c r="DG7" s="0"/>
+      <c r="DH7" s="0"/>
+      <c r="DI7" s="0"/>
+      <c r="DJ7" s="0"/>
+      <c r="DK7" s="0"/>
+      <c r="DL7" s="0"/>
+      <c r="DM7" s="0"/>
+      <c r="DN7" s="0"/>
+      <c r="DO7" s="0"/>
+      <c r="DP7" s="0"/>
+      <c r="DQ7" s="0"/>
+      <c r="DR7" s="0"/>
+      <c r="DS7" s="0"/>
+      <c r="DT7" s="0"/>
+      <c r="DU7" s="0"/>
+      <c r="DV7" s="0"/>
+      <c r="DW7" s="0"/>
+      <c r="DX7" s="0"/>
+      <c r="DY7" s="0"/>
+      <c r="DZ7" s="0"/>
+      <c r="EA7" s="0"/>
+      <c r="EB7" s="0"/>
+      <c r="EC7" s="0"/>
+      <c r="ED7" s="0"/>
+      <c r="EE7" s="0"/>
+      <c r="EF7" s="0"/>
+      <c r="EG7" s="0"/>
+      <c r="EH7" s="0"/>
+      <c r="EI7" s="0"/>
+      <c r="EJ7" s="0"/>
+      <c r="EK7" s="0"/>
+      <c r="EL7" s="0"/>
+      <c r="EM7" s="0"/>
+      <c r="EN7" s="0"/>
+      <c r="EO7" s="0"/>
+      <c r="EP7" s="0"/>
+      <c r="EQ7" s="0"/>
+      <c r="ER7" s="0"/>
+      <c r="ES7" s="0"/>
+      <c r="ET7" s="0"/>
+      <c r="EU7" s="0"/>
+      <c r="EV7" s="0"/>
+      <c r="EW7" s="0"/>
+      <c r="EX7" s="0"/>
+      <c r="EY7" s="0"/>
+      <c r="EZ7" s="0"/>
+      <c r="FA7" s="0"/>
+      <c r="FB7" s="0"/>
+      <c r="FC7" s="0"/>
+      <c r="FD7" s="0"/>
+      <c r="FE7" s="0"/>
+      <c r="FF7" s="0"/>
+      <c r="FG7" s="0"/>
+      <c r="FH7" s="0"/>
+      <c r="FI7" s="0"/>
+      <c r="FJ7" s="0"/>
+      <c r="FK7" s="0"/>
+      <c r="FL7" s="0"/>
+      <c r="FM7" s="0"/>
+      <c r="FN7" s="0"/>
+      <c r="FO7" s="0"/>
+      <c r="FP7" s="0"/>
+      <c r="FQ7" s="0"/>
+      <c r="FR7" s="0"/>
+      <c r="FS7" s="0"/>
+      <c r="FT7" s="0"/>
+      <c r="FU7" s="0"/>
+      <c r="FV7" s="0"/>
+      <c r="FW7" s="0"/>
+      <c r="FX7" s="0"/>
+      <c r="FY7" s="0"/>
+      <c r="FZ7" s="0"/>
+      <c r="GA7" s="0"/>
+      <c r="GB7" s="0"/>
+      <c r="GC7" s="0"/>
+      <c r="GD7" s="0"/>
+      <c r="GE7" s="0"/>
+      <c r="GF7" s="0"/>
+      <c r="GG7" s="0"/>
+      <c r="GH7" s="0"/>
+      <c r="GI7" s="0"/>
+      <c r="GJ7" s="0"/>
+      <c r="GK7" s="0"/>
+      <c r="GL7" s="0"/>
+      <c r="GM7" s="0"/>
+      <c r="GN7" s="0"/>
+      <c r="GO7" s="0"/>
+      <c r="GP7" s="0"/>
+      <c r="GQ7" s="0"/>
+      <c r="GR7" s="0"/>
+      <c r="GS7" s="0"/>
+      <c r="GT7" s="0"/>
+      <c r="GU7" s="0"/>
+      <c r="GV7" s="0"/>
+      <c r="GW7" s="0"/>
+      <c r="GX7" s="0"/>
+      <c r="GY7" s="0"/>
+      <c r="GZ7" s="0"/>
+      <c r="HA7" s="0"/>
+      <c r="HB7" s="0"/>
+      <c r="HC7" s="0"/>
+      <c r="HD7" s="0"/>
+      <c r="HE7" s="0"/>
+      <c r="HF7" s="0"/>
+      <c r="HG7" s="0"/>
+      <c r="HH7" s="0"/>
+      <c r="HI7" s="0"/>
+      <c r="HJ7" s="0"/>
+      <c r="HK7" s="0"/>
+      <c r="HL7" s="0"/>
+      <c r="HM7" s="0"/>
+      <c r="HN7" s="0"/>
+      <c r="HO7" s="0"/>
+      <c r="HP7" s="0"/>
+      <c r="HQ7" s="0"/>
+      <c r="HR7" s="0"/>
+      <c r="HS7" s="0"/>
+      <c r="HT7" s="0"/>
+      <c r="HU7" s="0"/>
+      <c r="HV7" s="0"/>
+      <c r="HW7" s="0"/>
+      <c r="HX7" s="0"/>
+      <c r="HY7" s="0"/>
+      <c r="HZ7" s="0"/>
+      <c r="IA7" s="0"/>
+      <c r="IB7" s="0"/>
+      <c r="IC7" s="0"/>
+      <c r="ID7" s="0"/>
+      <c r="IE7" s="0"/>
+      <c r="IF7" s="0"/>
+      <c r="IG7" s="0"/>
+      <c r="IH7" s="0"/>
+      <c r="II7" s="0"/>
+      <c r="IJ7" s="0"/>
+      <c r="IK7" s="0"/>
+      <c r="IL7" s="0"/>
+      <c r="IM7" s="0"/>
+      <c r="IN7" s="0"/>
+      <c r="IO7" s="0"/>
+      <c r="IP7" s="0"/>
+      <c r="IQ7" s="0"/>
+      <c r="IR7" s="0"/>
+      <c r="IS7" s="0"/>
+      <c r="IT7" s="0"/>
+      <c r="IU7" s="0"/>
+      <c r="IV7" s="0"/>
+      <c r="IW7" s="0"/>
+      <c r="IX7" s="0"/>
+      <c r="IY7" s="0"/>
+      <c r="IZ7" s="0"/>
+      <c r="JA7" s="0"/>
+      <c r="JB7" s="0"/>
+      <c r="JC7" s="0"/>
+      <c r="JD7" s="0"/>
+      <c r="JE7" s="0"/>
+      <c r="JF7" s="0"/>
+      <c r="JG7" s="0"/>
+      <c r="JH7" s="0"/>
+      <c r="JI7" s="0"/>
+      <c r="JJ7" s="0"/>
+      <c r="JK7" s="0"/>
+      <c r="JL7" s="0"/>
+      <c r="JM7" s="0"/>
+      <c r="JN7" s="0"/>
+      <c r="JO7" s="0"/>
+      <c r="JP7" s="0"/>
+      <c r="JQ7" s="0"/>
+      <c r="JR7" s="0"/>
+      <c r="JS7" s="0"/>
+      <c r="JT7" s="0"/>
+      <c r="JU7" s="0"/>
+      <c r="JV7" s="0"/>
+      <c r="JW7" s="0"/>
+      <c r="JX7" s="0"/>
+      <c r="JY7" s="0"/>
+      <c r="JZ7" s="0"/>
+      <c r="KA7" s="0"/>
+      <c r="KB7" s="0"/>
+      <c r="KC7" s="0"/>
+      <c r="KD7" s="0"/>
+      <c r="KE7" s="0"/>
+      <c r="KF7" s="0"/>
+      <c r="KG7" s="0"/>
+      <c r="KH7" s="0"/>
+      <c r="KI7" s="0"/>
+      <c r="KJ7" s="0"/>
+      <c r="KK7" s="0"/>
+      <c r="KL7" s="0"/>
+      <c r="KM7" s="0"/>
+      <c r="KN7" s="0"/>
+      <c r="KO7" s="0"/>
+      <c r="KP7" s="0"/>
+      <c r="KQ7" s="0"/>
+      <c r="KR7" s="0"/>
+      <c r="KS7" s="0"/>
+      <c r="KT7" s="0"/>
+      <c r="KU7" s="0"/>
+      <c r="KV7" s="0"/>
+      <c r="KW7" s="0"/>
+      <c r="KX7" s="0"/>
+      <c r="KY7" s="0"/>
+      <c r="KZ7" s="0"/>
+      <c r="LA7" s="0"/>
+      <c r="LB7" s="0"/>
+      <c r="LC7" s="0"/>
+      <c r="LD7" s="0"/>
+      <c r="LE7" s="0"/>
+      <c r="LF7" s="0"/>
+      <c r="LG7" s="0"/>
+      <c r="LH7" s="0"/>
+      <c r="LI7" s="0"/>
+      <c r="LJ7" s="0"/>
+      <c r="LK7" s="0"/>
+      <c r="LL7" s="0"/>
+      <c r="LM7" s="0"/>
+      <c r="LN7" s="0"/>
+      <c r="LO7" s="0"/>
+      <c r="LP7" s="0"/>
+      <c r="LQ7" s="0"/>
+      <c r="LR7" s="0"/>
+      <c r="LS7" s="0"/>
+      <c r="LT7" s="0"/>
+      <c r="LU7" s="0"/>
+      <c r="LV7" s="0"/>
+      <c r="LW7" s="0"/>
+      <c r="LX7" s="0"/>
+      <c r="LY7" s="0"/>
+      <c r="LZ7" s="0"/>
+      <c r="MA7" s="0"/>
+      <c r="MB7" s="0"/>
+      <c r="MC7" s="0"/>
+      <c r="MD7" s="0"/>
+      <c r="ME7" s="0"/>
+      <c r="MF7" s="0"/>
+      <c r="MG7" s="0"/>
+      <c r="MH7" s="0"/>
+      <c r="MI7" s="0"/>
+      <c r="MJ7" s="0"/>
+      <c r="MK7" s="0"/>
+      <c r="ML7" s="0"/>
+      <c r="MM7" s="0"/>
+      <c r="MN7" s="0"/>
+      <c r="MO7" s="0"/>
+      <c r="MP7" s="0"/>
+      <c r="MQ7" s="0"/>
+      <c r="MR7" s="0"/>
+      <c r="MS7" s="0"/>
+      <c r="MT7" s="0"/>
+      <c r="MU7" s="0"/>
+      <c r="MV7" s="0"/>
+      <c r="MW7" s="0"/>
+      <c r="MX7" s="0"/>
+      <c r="MY7" s="0"/>
+      <c r="MZ7" s="0"/>
+      <c r="NA7" s="0"/>
+      <c r="NB7" s="0"/>
+      <c r="NC7" s="0"/>
+      <c r="ND7" s="0"/>
+      <c r="NE7" s="0"/>
+      <c r="NF7" s="0"/>
+      <c r="NG7" s="0"/>
+      <c r="NH7" s="0"/>
+      <c r="NI7" s="0"/>
+      <c r="NJ7" s="0"/>
+      <c r="NK7" s="0"/>
+      <c r="NL7" s="0"/>
+      <c r="NM7" s="0"/>
+      <c r="NN7" s="0"/>
+      <c r="NO7" s="0"/>
+      <c r="NP7" s="0"/>
+      <c r="NQ7" s="0"/>
+      <c r="NR7" s="0"/>
+      <c r="NS7" s="0"/>
+      <c r="NT7" s="0"/>
+      <c r="NU7" s="0"/>
+      <c r="NV7" s="0"/>
+      <c r="NW7" s="0"/>
+      <c r="NX7" s="0"/>
+      <c r="NY7" s="0"/>
+      <c r="NZ7" s="0"/>
+      <c r="OA7" s="0"/>
+      <c r="OB7" s="0"/>
+      <c r="OC7" s="0"/>
+      <c r="OD7" s="0"/>
+      <c r="OE7" s="0"/>
+      <c r="OF7" s="0"/>
+      <c r="OG7" s="0"/>
+      <c r="OH7" s="0"/>
+      <c r="OI7" s="0"/>
+      <c r="OJ7" s="0"/>
+      <c r="OK7" s="0"/>
+      <c r="OL7" s="0"/>
+      <c r="OM7" s="0"/>
+      <c r="ON7" s="0"/>
+      <c r="OO7" s="0"/>
+      <c r="OP7" s="0"/>
+      <c r="OQ7" s="0"/>
+      <c r="OR7" s="0"/>
+      <c r="OS7" s="0"/>
+      <c r="OT7" s="0"/>
+      <c r="OU7" s="0"/>
+      <c r="OV7" s="0"/>
+      <c r="OW7" s="0"/>
+      <c r="OX7" s="0"/>
+      <c r="OY7" s="0"/>
+      <c r="OZ7" s="0"/>
+      <c r="PA7" s="0"/>
+      <c r="PB7" s="0"/>
+      <c r="PC7" s="0"/>
+      <c r="PD7" s="0"/>
+      <c r="PE7" s="0"/>
+      <c r="PF7" s="0"/>
+      <c r="PG7" s="0"/>
+      <c r="PH7" s="0"/>
+      <c r="PI7" s="0"/>
+      <c r="PJ7" s="0"/>
+      <c r="PK7" s="0"/>
+      <c r="PL7" s="0"/>
+      <c r="PM7" s="0"/>
+      <c r="PN7" s="0"/>
+      <c r="PO7" s="0"/>
+      <c r="PP7" s="0"/>
+      <c r="PQ7" s="0"/>
+      <c r="PR7" s="0"/>
+      <c r="PS7" s="0"/>
+      <c r="PT7" s="0"/>
+      <c r="PU7" s="0"/>
+      <c r="PV7" s="0"/>
+      <c r="PW7" s="0"/>
+      <c r="PX7" s="0"/>
+      <c r="PY7" s="0"/>
+      <c r="PZ7" s="0"/>
+      <c r="QA7" s="0"/>
+      <c r="QB7" s="0"/>
+      <c r="QC7" s="0"/>
+      <c r="QD7" s="0"/>
+      <c r="QE7" s="0"/>
+      <c r="QF7" s="0"/>
+      <c r="QG7" s="0"/>
+      <c r="QH7" s="0"/>
+      <c r="QI7" s="0"/>
+      <c r="QJ7" s="0"/>
+      <c r="QK7" s="0"/>
+      <c r="QL7" s="0"/>
+      <c r="QM7" s="0"/>
+      <c r="QN7" s="0"/>
+      <c r="QO7" s="0"/>
+      <c r="QP7" s="0"/>
+      <c r="QQ7" s="0"/>
+      <c r="QR7" s="0"/>
+      <c r="QS7" s="0"/>
+      <c r="QT7" s="0"/>
+      <c r="QU7" s="0"/>
+      <c r="QV7" s="0"/>
+      <c r="QW7" s="0"/>
+      <c r="QX7" s="0"/>
+      <c r="QY7" s="0"/>
+      <c r="QZ7" s="0"/>
+      <c r="RA7" s="0"/>
+      <c r="RB7" s="0"/>
+      <c r="RC7" s="0"/>
+      <c r="RD7" s="0"/>
+      <c r="RE7" s="0"/>
+      <c r="RF7" s="0"/>
+      <c r="RG7" s="0"/>
+      <c r="RH7" s="0"/>
+      <c r="RI7" s="0"/>
+      <c r="RJ7" s="0"/>
+      <c r="RK7" s="0"/>
+      <c r="RL7" s="0"/>
+      <c r="RM7" s="0"/>
+      <c r="RN7" s="0"/>
+      <c r="RO7" s="0"/>
+      <c r="RP7" s="0"/>
+      <c r="RQ7" s="0"/>
+      <c r="RR7" s="0"/>
+      <c r="RS7" s="0"/>
+      <c r="RT7" s="0"/>
+      <c r="RU7" s="0"/>
+      <c r="RV7" s="0"/>
+      <c r="RW7" s="0"/>
+      <c r="RX7" s="0"/>
+      <c r="RY7" s="0"/>
+      <c r="RZ7" s="0"/>
+      <c r="SA7" s="0"/>
+      <c r="SB7" s="0"/>
+      <c r="SC7" s="0"/>
+      <c r="SD7" s="0"/>
+      <c r="SE7" s="0"/>
+      <c r="SF7" s="0"/>
+      <c r="SG7" s="0"/>
+      <c r="SH7" s="0"/>
+      <c r="SI7" s="0"/>
+      <c r="SJ7" s="0"/>
+      <c r="SK7" s="0"/>
+      <c r="SL7" s="0"/>
+      <c r="SM7" s="0"/>
+      <c r="SN7" s="0"/>
+      <c r="SO7" s="0"/>
+      <c r="SP7" s="0"/>
+      <c r="SQ7" s="0"/>
+      <c r="SR7" s="0"/>
+      <c r="SS7" s="0"/>
+      <c r="ST7" s="0"/>
+      <c r="SU7" s="0"/>
+      <c r="SV7" s="0"/>
+      <c r="SW7" s="0"/>
+      <c r="SX7" s="0"/>
+      <c r="SY7" s="0"/>
+      <c r="SZ7" s="0"/>
+      <c r="TA7" s="0"/>
+      <c r="TB7" s="0"/>
+      <c r="TC7" s="0"/>
+      <c r="TD7" s="0"/>
+      <c r="TE7" s="0"/>
+      <c r="TF7" s="0"/>
+      <c r="TG7" s="0"/>
+      <c r="TH7" s="0"/>
+      <c r="TI7" s="0"/>
+      <c r="TJ7" s="0"/>
+      <c r="TK7" s="0"/>
+      <c r="TL7" s="0"/>
+      <c r="TM7" s="0"/>
+      <c r="TN7" s="0"/>
+      <c r="TO7" s="0"/>
+      <c r="TP7" s="0"/>
+      <c r="TQ7" s="0"/>
+      <c r="TR7" s="0"/>
+      <c r="TS7" s="0"/>
+      <c r="TT7" s="0"/>
+      <c r="TU7" s="0"/>
+      <c r="TV7" s="0"/>
+      <c r="TW7" s="0"/>
+      <c r="TX7" s="0"/>
+      <c r="TY7" s="0"/>
+      <c r="TZ7" s="0"/>
+      <c r="UA7" s="0"/>
+      <c r="UB7" s="0"/>
+      <c r="UC7" s="0"/>
+      <c r="UD7" s="0"/>
+      <c r="UE7" s="0"/>
+      <c r="UF7" s="0"/>
+      <c r="UG7" s="0"/>
+      <c r="UH7" s="0"/>
+      <c r="UI7" s="0"/>
+      <c r="UJ7" s="0"/>
+      <c r="UK7" s="0"/>
+      <c r="UL7" s="0"/>
+      <c r="UM7" s="0"/>
+      <c r="UN7" s="0"/>
+      <c r="UO7" s="0"/>
+      <c r="UP7" s="0"/>
+      <c r="UQ7" s="0"/>
+      <c r="UR7" s="0"/>
+      <c r="US7" s="0"/>
+      <c r="UT7" s="0"/>
+      <c r="UU7" s="0"/>
+      <c r="UV7" s="0"/>
+      <c r="UW7" s="0"/>
+      <c r="UX7" s="0"/>
+      <c r="UY7" s="0"/>
+      <c r="UZ7" s="0"/>
+      <c r="VA7" s="0"/>
+      <c r="VB7" s="0"/>
+      <c r="VC7" s="0"/>
+      <c r="VD7" s="0"/>
+      <c r="VE7" s="0"/>
+      <c r="VF7" s="0"/>
+      <c r="VG7" s="0"/>
+      <c r="VH7" s="0"/>
+      <c r="VI7" s="0"/>
+      <c r="VJ7" s="0"/>
+      <c r="VK7" s="0"/>
+      <c r="VL7" s="0"/>
+      <c r="VM7" s="0"/>
+      <c r="VN7" s="0"/>
+      <c r="VO7" s="0"/>
+      <c r="VP7" s="0"/>
+      <c r="VQ7" s="0"/>
+      <c r="VR7" s="0"/>
+      <c r="VS7" s="0"/>
+      <c r="VT7" s="0"/>
+      <c r="VU7" s="0"/>
+      <c r="VV7" s="0"/>
+      <c r="VW7" s="0"/>
+      <c r="VX7" s="0"/>
+      <c r="VY7" s="0"/>
+      <c r="VZ7" s="0"/>
+      <c r="WA7" s="0"/>
+      <c r="WB7" s="0"/>
+      <c r="WC7" s="0"/>
+      <c r="WD7" s="0"/>
+      <c r="WE7" s="0"/>
+      <c r="WF7" s="0"/>
+      <c r="WG7" s="0"/>
+      <c r="WH7" s="0"/>
+      <c r="WI7" s="0"/>
+      <c r="WJ7" s="0"/>
+      <c r="WK7" s="0"/>
+      <c r="WL7" s="0"/>
+      <c r="WM7" s="0"/>
+      <c r="WN7" s="0"/>
+      <c r="WO7" s="0"/>
+      <c r="WP7" s="0"/>
+      <c r="WQ7" s="0"/>
+      <c r="WR7" s="0"/>
+      <c r="WS7" s="0"/>
+      <c r="WT7" s="0"/>
+      <c r="WU7" s="0"/>
+      <c r="WV7" s="0"/>
+      <c r="WW7" s="0"/>
+      <c r="WX7" s="0"/>
+      <c r="WY7" s="0"/>
+      <c r="WZ7" s="0"/>
+      <c r="XA7" s="0"/>
+      <c r="XB7" s="0"/>
+      <c r="XC7" s="0"/>
+      <c r="XD7" s="0"/>
+      <c r="XE7" s="0"/>
+      <c r="XF7" s="0"/>
+      <c r="XG7" s="0"/>
+      <c r="XH7" s="0"/>
+      <c r="XI7" s="0"/>
+      <c r="XJ7" s="0"/>
+      <c r="XK7" s="0"/>
+      <c r="XL7" s="0"/>
+      <c r="XM7" s="0"/>
+      <c r="XN7" s="0"/>
+      <c r="XO7" s="0"/>
+      <c r="XP7" s="0"/>
+      <c r="XQ7" s="0"/>
+      <c r="XR7" s="0"/>
+      <c r="XS7" s="0"/>
+      <c r="XT7" s="0"/>
+      <c r="XU7" s="0"/>
+      <c r="XV7" s="0"/>
+      <c r="XW7" s="0"/>
+      <c r="XX7" s="0"/>
+      <c r="XY7" s="0"/>
+      <c r="XZ7" s="0"/>
+      <c r="YA7" s="0"/>
+      <c r="YB7" s="0"/>
+      <c r="YC7" s="0"/>
+      <c r="YD7" s="0"/>
+      <c r="YE7" s="0"/>
+      <c r="YF7" s="0"/>
+      <c r="YG7" s="0"/>
+      <c r="YH7" s="0"/>
+      <c r="YI7" s="0"/>
+      <c r="YJ7" s="0"/>
+      <c r="YK7" s="0"/>
+      <c r="YL7" s="0"/>
+      <c r="YM7" s="0"/>
+      <c r="YN7" s="0"/>
+      <c r="YO7" s="0"/>
+      <c r="YP7" s="0"/>
+      <c r="YQ7" s="0"/>
+      <c r="YR7" s="0"/>
+      <c r="YS7" s="0"/>
+      <c r="YT7" s="0"/>
+      <c r="YU7" s="0"/>
+      <c r="YV7" s="0"/>
+      <c r="YW7" s="0"/>
+      <c r="YX7" s="0"/>
+      <c r="YY7" s="0"/>
+      <c r="YZ7" s="0"/>
+      <c r="ZA7" s="0"/>
+      <c r="ZB7" s="0"/>
+      <c r="ZC7" s="0"/>
+      <c r="ZD7" s="0"/>
+      <c r="ZE7" s="0"/>
+      <c r="ZF7" s="0"/>
+      <c r="ZG7" s="0"/>
+      <c r="ZH7" s="0"/>
+      <c r="ZI7" s="0"/>
+      <c r="ZJ7" s="0"/>
+      <c r="ZK7" s="0"/>
+      <c r="ZL7" s="0"/>
+      <c r="ZM7" s="0"/>
+      <c r="ZN7" s="0"/>
+      <c r="ZO7" s="0"/>
+      <c r="ZP7" s="0"/>
+      <c r="ZQ7" s="0"/>
+      <c r="ZR7" s="0"/>
+      <c r="ZS7" s="0"/>
+      <c r="ZT7" s="0"/>
+      <c r="ZU7" s="0"/>
+      <c r="ZV7" s="0"/>
+      <c r="ZW7" s="0"/>
+      <c r="ZX7" s="0"/>
+      <c r="ZY7" s="0"/>
+      <c r="ZZ7" s="0"/>
+      <c r="AAA7" s="0"/>
+      <c r="AAB7" s="0"/>
+      <c r="AAC7" s="0"/>
+      <c r="AAD7" s="0"/>
+      <c r="AAE7" s="0"/>
+      <c r="AAF7" s="0"/>
+      <c r="AAG7" s="0"/>
+      <c r="AAH7" s="0"/>
+      <c r="AAI7" s="0"/>
+      <c r="AAJ7" s="0"/>
+      <c r="AAK7" s="0"/>
+      <c r="AAL7" s="0"/>
+      <c r="AAM7" s="0"/>
+      <c r="AAN7" s="0"/>
+      <c r="AAO7" s="0"/>
+      <c r="AAP7" s="0"/>
+      <c r="AAQ7" s="0"/>
+      <c r="AAR7" s="0"/>
+      <c r="AAS7" s="0"/>
+      <c r="AAT7" s="0"/>
+      <c r="AAU7" s="0"/>
+      <c r="AAV7" s="0"/>
+      <c r="AAW7" s="0"/>
+      <c r="AAX7" s="0"/>
+      <c r="AAY7" s="0"/>
+      <c r="AAZ7" s="0"/>
+      <c r="ABA7" s="0"/>
+      <c r="ABB7" s="0"/>
+      <c r="ABC7" s="0"/>
+      <c r="ABD7" s="0"/>
+      <c r="ABE7" s="0"/>
+      <c r="ABF7" s="0"/>
+      <c r="ABG7" s="0"/>
+      <c r="ABH7" s="0"/>
+      <c r="ABI7" s="0"/>
+      <c r="ABJ7" s="0"/>
+      <c r="ABK7" s="0"/>
+      <c r="ABL7" s="0"/>
+      <c r="ABM7" s="0"/>
+      <c r="ABN7" s="0"/>
+      <c r="ABO7" s="0"/>
+      <c r="ABP7" s="0"/>
+      <c r="ABQ7" s="0"/>
+      <c r="ABR7" s="0"/>
+      <c r="ABS7" s="0"/>
+      <c r="ABT7" s="0"/>
+      <c r="ABU7" s="0"/>
+      <c r="ABV7" s="0"/>
+      <c r="ABW7" s="0"/>
+      <c r="ABX7" s="0"/>
+      <c r="ABY7" s="0"/>
+      <c r="ABZ7" s="0"/>
+      <c r="ACA7" s="0"/>
+      <c r="ACB7" s="0"/>
+      <c r="ACC7" s="0"/>
+      <c r="ACD7" s="0"/>
+      <c r="ACE7" s="0"/>
+      <c r="ACF7" s="0"/>
+      <c r="ACG7" s="0"/>
+      <c r="ACH7" s="0"/>
+      <c r="ACI7" s="0"/>
+      <c r="ACJ7" s="0"/>
+      <c r="ACK7" s="0"/>
+      <c r="ACL7" s="0"/>
+      <c r="ACM7" s="0"/>
+      <c r="ACN7" s="0"/>
+      <c r="ACO7" s="0"/>
+      <c r="ACP7" s="0"/>
+      <c r="ACQ7" s="0"/>
+      <c r="ACR7" s="0"/>
+      <c r="ACS7" s="0"/>
+      <c r="ACT7" s="0"/>
+      <c r="ACU7" s="0"/>
+      <c r="ACV7" s="0"/>
+      <c r="ACW7" s="0"/>
+      <c r="ACX7" s="0"/>
+      <c r="ACY7" s="0"/>
+      <c r="ACZ7" s="0"/>
+      <c r="ADA7" s="0"/>
+      <c r="ADB7" s="0"/>
+      <c r="ADC7" s="0"/>
+      <c r="ADD7" s="0"/>
+      <c r="ADE7" s="0"/>
+      <c r="ADF7" s="0"/>
+      <c r="ADG7" s="0"/>
+      <c r="ADH7" s="0"/>
+      <c r="ADI7" s="0"/>
+      <c r="ADJ7" s="0"/>
+      <c r="ADK7" s="0"/>
+      <c r="ADL7" s="0"/>
+      <c r="ADM7" s="0"/>
+      <c r="ADN7" s="0"/>
+      <c r="ADO7" s="0"/>
+      <c r="ADP7" s="0"/>
+      <c r="ADQ7" s="0"/>
+      <c r="ADR7" s="0"/>
+      <c r="ADS7" s="0"/>
+      <c r="ADT7" s="0"/>
+      <c r="ADU7" s="0"/>
+      <c r="ADV7" s="0"/>
+      <c r="ADW7" s="0"/>
+      <c r="ADX7" s="0"/>
+      <c r="ADY7" s="0"/>
+      <c r="ADZ7" s="0"/>
+      <c r="AEA7" s="0"/>
+      <c r="AEB7" s="0"/>
+      <c r="AEC7" s="0"/>
+      <c r="AED7" s="0"/>
+      <c r="AEE7" s="0"/>
+      <c r="AEF7" s="0"/>
+      <c r="AEG7" s="0"/>
+      <c r="AEH7" s="0"/>
+      <c r="AEI7" s="0"/>
+      <c r="AEJ7" s="0"/>
+      <c r="AEK7" s="0"/>
+      <c r="AEL7" s="0"/>
+      <c r="AEM7" s="0"/>
+      <c r="AEN7" s="0"/>
+      <c r="AEO7" s="0"/>
+      <c r="AEP7" s="0"/>
+      <c r="AEQ7" s="0"/>
+      <c r="AER7" s="0"/>
+      <c r="AES7" s="0"/>
+      <c r="AET7" s="0"/>
+      <c r="AEU7" s="0"/>
+      <c r="AEV7" s="0"/>
+      <c r="AEW7" s="0"/>
+      <c r="AEX7" s="0"/>
+      <c r="AEY7" s="0"/>
+      <c r="AEZ7" s="0"/>
+      <c r="AFA7" s="0"/>
+      <c r="AFB7" s="0"/>
+      <c r="AFC7" s="0"/>
+      <c r="AFD7" s="0"/>
+      <c r="AFE7" s="0"/>
+      <c r="AFF7" s="0"/>
+      <c r="AFG7" s="0"/>
+      <c r="AFH7" s="0"/>
+      <c r="AFI7" s="0"/>
+      <c r="AFJ7" s="0"/>
+      <c r="AFK7" s="0"/>
+      <c r="AFL7" s="0"/>
+      <c r="AFM7" s="0"/>
+      <c r="AFN7" s="0"/>
+      <c r="AFO7" s="0"/>
+      <c r="AFP7" s="0"/>
+      <c r="AFQ7" s="0"/>
+      <c r="AFR7" s="0"/>
+      <c r="AFS7" s="0"/>
+      <c r="AFT7" s="0"/>
+      <c r="AFU7" s="0"/>
+      <c r="AFV7" s="0"/>
+      <c r="AFW7" s="0"/>
+      <c r="AFX7" s="0"/>
+      <c r="AFY7" s="0"/>
+      <c r="AFZ7" s="0"/>
+      <c r="AGA7" s="0"/>
+      <c r="AGB7" s="0"/>
+      <c r="AGC7" s="0"/>
+      <c r="AGD7" s="0"/>
+      <c r="AGE7" s="0"/>
+      <c r="AGF7" s="0"/>
+      <c r="AGG7" s="0"/>
+      <c r="AGH7" s="0"/>
+      <c r="AGI7" s="0"/>
+      <c r="AGJ7" s="0"/>
+      <c r="AGK7" s="0"/>
+      <c r="AGL7" s="0"/>
+      <c r="AGM7" s="0"/>
+      <c r="AGN7" s="0"/>
+      <c r="AGO7" s="0"/>
+      <c r="AGP7" s="0"/>
+      <c r="AGQ7" s="0"/>
+      <c r="AGR7" s="0"/>
+      <c r="AGS7" s="0"/>
+      <c r="AGT7" s="0"/>
+      <c r="AGU7" s="0"/>
+      <c r="AGV7" s="0"/>
+      <c r="AGW7" s="0"/>
+      <c r="AGX7" s="0"/>
+      <c r="AGY7" s="0"/>
+      <c r="AGZ7" s="0"/>
+      <c r="AHA7" s="0"/>
+      <c r="AHB7" s="0"/>
+      <c r="AHC7" s="0"/>
+      <c r="AHD7" s="0"/>
+      <c r="AHE7" s="0"/>
+      <c r="AHF7" s="0"/>
+      <c r="AHG7" s="0"/>
+      <c r="AHH7" s="0"/>
+      <c r="AHI7" s="0"/>
+      <c r="AHJ7" s="0"/>
+      <c r="AHK7" s="0"/>
+      <c r="AHL7" s="0"/>
+      <c r="AHM7" s="0"/>
+      <c r="AHN7" s="0"/>
+      <c r="AHO7" s="0"/>
+      <c r="AHP7" s="0"/>
+      <c r="AHQ7" s="0"/>
+      <c r="AHR7" s="0"/>
+      <c r="AHS7" s="0"/>
+      <c r="AHT7" s="0"/>
+      <c r="AHU7" s="0"/>
+      <c r="AHV7" s="0"/>
+      <c r="AHW7" s="0"/>
+      <c r="AHX7" s="0"/>
+      <c r="AHY7" s="0"/>
+      <c r="AHZ7" s="0"/>
+      <c r="AIA7" s="0"/>
+      <c r="AIB7" s="0"/>
+      <c r="AIC7" s="0"/>
+      <c r="AID7" s="0"/>
+      <c r="AIE7" s="0"/>
+      <c r="AIF7" s="0"/>
+      <c r="AIG7" s="0"/>
+      <c r="AIH7" s="0"/>
+      <c r="AII7" s="0"/>
+      <c r="AIJ7" s="0"/>
+      <c r="AIK7" s="0"/>
+      <c r="AIL7" s="0"/>
+      <c r="AIM7" s="0"/>
+      <c r="AIN7" s="0"/>
+      <c r="AIO7" s="0"/>
+      <c r="AIP7" s="0"/>
+      <c r="AIQ7" s="0"/>
+      <c r="AIR7" s="0"/>
+      <c r="AIS7" s="0"/>
+      <c r="AIT7" s="0"/>
+      <c r="AIU7" s="0"/>
+      <c r="AIV7" s="0"/>
+      <c r="AIW7" s="0"/>
+      <c r="AIX7" s="0"/>
+      <c r="AIY7" s="0"/>
+      <c r="AIZ7" s="0"/>
+      <c r="AJA7" s="0"/>
+      <c r="AJB7" s="0"/>
+      <c r="AJC7" s="0"/>
+      <c r="AJD7" s="0"/>
+      <c r="AJE7" s="0"/>
+      <c r="AJF7" s="0"/>
+      <c r="AJG7" s="0"/>
+      <c r="AJH7" s="0"/>
+      <c r="AJI7" s="0"/>
+      <c r="AJJ7" s="0"/>
+      <c r="AJK7" s="0"/>
+      <c r="AJL7" s="0"/>
+      <c r="AJM7" s="0"/>
+      <c r="AJN7" s="0"/>
+      <c r="AJO7" s="0"/>
+      <c r="AJP7" s="0"/>
+      <c r="AJQ7" s="0"/>
+      <c r="AJR7" s="0"/>
+      <c r="AJS7" s="0"/>
+      <c r="AJT7" s="0"/>
+      <c r="AJU7" s="0"/>
+      <c r="AJV7" s="0"/>
+      <c r="AJW7" s="0"/>
+      <c r="AJX7" s="0"/>
+      <c r="AJY7" s="0"/>
+      <c r="AJZ7" s="0"/>
+      <c r="AKA7" s="0"/>
+      <c r="AKB7" s="0"/>
+      <c r="AKC7" s="0"/>
+      <c r="AKD7" s="0"/>
+      <c r="AKE7" s="0"/>
+      <c r="AKF7" s="0"/>
+      <c r="AKG7" s="0"/>
+      <c r="AKH7" s="0"/>
+      <c r="AKI7" s="0"/>
+      <c r="AKJ7" s="0"/>
+      <c r="AKK7" s="0"/>
+      <c r="AKL7" s="0"/>
+      <c r="AKM7" s="0"/>
+      <c r="AKN7" s="0"/>
+      <c r="AKO7" s="0"/>
+      <c r="AKP7" s="0"/>
+      <c r="AKQ7" s="0"/>
+      <c r="AKR7" s="0"/>
+      <c r="AKS7" s="0"/>
+      <c r="AKT7" s="0"/>
+      <c r="AKU7" s="0"/>
+      <c r="AKV7" s="0"/>
+      <c r="AKW7" s="0"/>
+      <c r="AKX7" s="0"/>
+      <c r="AKY7" s="0"/>
+      <c r="AKZ7" s="0"/>
+      <c r="ALA7" s="0"/>
+      <c r="ALB7" s="0"/>
+      <c r="ALC7" s="0"/>
+      <c r="ALD7" s="0"/>
+      <c r="ALE7" s="0"/>
+      <c r="ALF7" s="0"/>
+      <c r="ALG7" s="0"/>
+      <c r="ALH7" s="0"/>
+      <c r="ALI7" s="0"/>
+      <c r="ALJ7" s="0"/>
+      <c r="ALK7" s="0"/>
+      <c r="ALL7" s="0"/>
+      <c r="ALM7" s="0"/>
+      <c r="ALN7" s="0"/>
+      <c r="ALO7" s="0"/>
+      <c r="ALP7" s="0"/>
+      <c r="ALQ7" s="0"/>
+      <c r="ALR7" s="0"/>
+      <c r="ALS7" s="0"/>
+      <c r="ALT7" s="0"/>
+      <c r="ALU7" s="0"/>
+      <c r="ALV7" s="0"/>
+      <c r="ALW7" s="0"/>
+      <c r="ALX7" s="0"/>
+      <c r="ALY7" s="0"/>
+      <c r="ALZ7" s="0"/>
+      <c r="AMA7" s="0"/>
+      <c r="AMB7" s="0"/>
+      <c r="AMC7" s="0"/>
+      <c r="AMD7" s="0"/>
+      <c r="AME7" s="0"/>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -612,47 +1648,47 @@
         <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,66 +1699,100 @@
         <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" s="1" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E12" s="1" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E13" s="1" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="1" t="n">
+      <c r="E15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>